<commit_message>
add test coverage for prepost.Simulations.ManTurb64
</commit_message>
<xml_diff>
--- a/wetb/prepost/tests/data/demo_dlc/ref/htc/DLCs/dlc01_demos.xlsx
+++ b/wetb/prepost/tests/data/demo_dlc/ref/htc/DLCs/dlc01_demos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
   <si>
     <t xml:space="preserve">[t0]</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t xml:space="preserve">hawc_binary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turb_s100_10ms</t>
   </si>
 </sst>
 </file>
@@ -294,46 +297,46 @@
   <dimension ref="A1:AM4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="Q16" activeCellId="0" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.1275510204082"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.7244897959184"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3418367346939"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.23469387755102"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="6.3469387755102"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="38" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="38" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -690,8 +693,8 @@
         <v>39</v>
       </c>
       <c r="D4" s="6" t="str">
-        <f aca="false">"dlc01_steady_wsp" &amp; E4 &amp; "_noturb"</f>
-        <v>dlc01_steady_wsp10_noturb</v>
+        <f aca="false">"dlc01_steady_wsp" &amp; E4 &amp; "_s100"</f>
+        <v>dlc01_steady_wsp10_s100</v>
       </c>
       <c r="E4" s="5" t="n">
         <f aca="false">E3+1</f>
@@ -701,21 +704,21 @@
         <v>0</v>
       </c>
       <c r="G4" s="5" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H4" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" s="7" t="n">
         <f aca="false">(0.16*(0.75*E4+5.6))/E4</f>
         <v>0.2096</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="K4" s="8" t="n">
-        <f aca="false">E4*B4/8192</f>
-        <v>0.048828125</v>
+        <f aca="false">E4*B4/512</f>
+        <v>0.78125</v>
       </c>
       <c r="L4" s="5" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
previous commit introduced bug, fixed and covered by extending test
</commit_message>
<xml_diff>
--- a/wetb/prepost/tests/data/demo_dlc/ref/htc/DLCs/dlc01_demos.xlsx
+++ b/wetb/prepost/tests/data/demo_dlc/ref/htc/DLCs/dlc01_demos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
   <si>
     <t xml:space="preserve">[t0]</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t xml:space="preserve">turb_s100_10ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turb_s101_11ms</t>
   </si>
 </sst>
 </file>
@@ -294,49 +297,49 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AM4"/>
+  <dimension ref="A1:AM5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q16" activeCellId="0" sqref="Q16"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.05102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.7244897959184"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.91326530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.3163265306122"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.0714285714286"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.530612244898"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.50510204081633"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="6.20918367346939"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="38" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -792,10 +795,122 @@
         <v>41</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="n">
+        <f aca="false">A4</f>
+        <v>20</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <f aca="false">A5+20</f>
+        <v>40</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="6" t="str">
+        <f aca="false">"dlc01_steady_wsp" &amp; E5 &amp; "_s101"</f>
+        <v>dlc01_steady_wsp11_s101</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <f aca="false">E4+1</f>
+        <v>11</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <v>100</v>
+      </c>
+      <c r="H5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" s="7" t="n">
+        <f aca="false">(0.16*(0.75*E5+5.6))/E5</f>
+        <v>0.201454545454545</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" s="8" t="n">
+        <f aca="false">E5*B5/512</f>
+        <v>0.859375</v>
+      </c>
+      <c r="L5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" s="9" t="n">
+        <f aca="false">8/E5</f>
+        <v>0.727272727272727</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="W5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="X5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y5" s="5" t="n">
+        <v>-1</v>
+      </c>
+      <c r="Z5" s="5" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AA5" s="5" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AB5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC5" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD5" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE5" s="5" t="n">
+        <v>5000</v>
+      </c>
+      <c r="AF5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG5" s="5" t="n">
+        <v>5000</v>
+      </c>
+      <c r="AH5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI5" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ5" s="5"/>
+      <c r="AK5" s="5" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AL5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AM5" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
dirty fix [tu_seed]/[seed] tags, need solution for issue #37 urgently
</commit_message>
<xml_diff>
--- a/wetb/prepost/tests/data/demo_dlc/ref/htc/DLCs/dlc01_demos.xlsx
+++ b/wetb/prepost/tests/data/demo_dlc/ref/htc/DLCs/dlc01_demos.xlsx
@@ -40,7 +40,7 @@
     <t xml:space="preserve">[wdir]</t>
   </si>
   <si>
-    <t xml:space="preserve">[tu_seed]</t>
+    <t xml:space="preserve">[seed]</t>
   </si>
   <si>
     <t xml:space="preserve">[tu_model]</t>
@@ -167,7 +167,7 @@
     <numFmt numFmtId="166" formatCode="0.000000"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -191,21 +191,144 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -213,8 +336,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -238,25 +376,73 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -281,14 +467,90 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="22">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -299,47 +561,49 @@
   </sheetPr>
   <dimension ref="A1:AM5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.91326530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.3163265306122"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="10.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="6.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="6.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="6.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="6.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="16.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="7.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="15.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="12.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="18.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="29" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="13.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="10.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="17.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="9.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="9.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="11.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="38" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>